<commit_message>
updated some session data and debugged webhook
</commit_message>
<xml_diff>
--- a/resources/Session Info - IBM - modified 5.7.22.xlsx
+++ b/resources/Session Info - IBM - modified 5.7.22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leighw/git/actiac/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28227736-10B4-D448-99B5-B2A00D89FE97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71085DE6-B329-FF4B-A43E-BB7E03E30D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25580" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,18 +100,12 @@
     <t>Breakout Session B</t>
   </si>
   <si>
-    <t>Discussing how AI capabilities can provide effective distillation of information at scale for improved and timely decision making.</t>
-  </si>
-  <si>
     <t>Driving Innovation to Support the Mission</t>
   </si>
   <si>
     <t>Breakout Session A</t>
   </si>
   <si>
-    <t>Innovation comes in many forms, including broth both process-orient and technical.  with budgets increasinly tight and an ever-expanding workload, government CXOs have become the drivers of innovation across the Federal enterprise.  Join us for adiscussion on how a diverse group of leaders from across government are working to foster a culture that promotes and rewards innovation, drives change, and benefits mission performance by empowering employees across their respective organizations.</t>
-  </si>
-  <si>
     <t>Key Executive Fireside Chat/Interview</t>
   </si>
   <si>
@@ -178,9 +172,6 @@
     <t>Why the Future of Government is a Citizen Experience</t>
   </si>
   <si>
-    <t>What if ROI was not in a spreadsheet or financial ledger, but it was the constituent experience and the satisfaction of a job done well. Not just well done even - amazingly done. We, with a partnership of industry and public sector, must focus on the experience of the actual people we need to serve and reduce the burden on our public sector workforce.  State governments are harnessing the momentum of change to focus on the citizen experience and enabling agencies to innovate and modernize the way we serve customers. State agencies are propelling the path to production, while Central IT is utilizing strategic technologies to empower agencies to act faster and mitigate the unforeseen risk inherent in IT operations.  How do we realize Public ROI? By removing the barriers to innovation, owning the hurdles that slow operations down and embracing the momentum of change.</t>
-  </si>
-  <si>
     <t>Choptank ABC</t>
   </si>
   <si>
@@ -229,9 +220,6 @@
     <t>End Time</t>
   </si>
   <si>
-    <t xml:space="preserve"> Location</t>
-  </si>
-  <si>
     <t>Session Type</t>
   </si>
   <si>
@@ -245,6 +233,18 @@
   </si>
   <si>
     <t>RockIT:  Going Beyond Security:  A Conversation on Digital Transformation and Digital Experience</t>
+  </si>
+  <si>
+    <t>Discussing how A I capabilities can provide effective distillation of information at scale for improved and timely decision making.</t>
+  </si>
+  <si>
+    <t>Innovation comes in many forms, including broth both process-orient and technical.  with budgets increasinly tight and an ever-expanding workload, government C X Os have become the drivers of innovation across the Federal enterprise.  Join us for adiscussion on how a diverse group of leaders from across government are working to foster a culture that promotes and rewards innovation, drives change, and benefits mission performance by empowering employees across their respective organizations.</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>What if R O I was not in a spreadsheet or financial ledger, but it was the constituent experience and the satisfaction of a job done well. Not just well done even - amazingly done. We, with a partnership of industry and public sector, must focus on the experience of the actual people we need to serve and reduce the burden on our public sector workforce.  State governments are harnessing the momentum of change to focus on the citizen experience and enabling agencies to innovate and modernize the way we serve customers. State agencies are propelling the path to production, while Central I T is utilizing strategic technologies to empower agencies to act faster and mitigate the unforeseen risk inherent in I T operations.  How do we realize Public R O I? By removing the barriers to innovation, owning the hurdles that slow operations down and embracing the momentum of change.</t>
   </si>
 </sst>
 </file>
@@ -616,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -633,31 +633,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="D1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -680,7 +680,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="32" x14ac:dyDescent="0.2">
@@ -706,7 +706,7 @@
       </c>
       <c r="H3" s="6"/>
       <c r="I3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -730,7 +730,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="6"/>
       <c r="I4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -756,7 +756,7 @@
         <v>6</v>
       </c>
       <c r="I5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -782,7 +782,7 @@
         <v>8</v>
       </c>
       <c r="I6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="48" x14ac:dyDescent="0.2">
@@ -810,7 +810,7 @@
         <v>8</v>
       </c>
       <c r="I7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -836,7 +836,7 @@
         <v>12</v>
       </c>
       <c r="I8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -862,7 +862,7 @@
         <v>12</v>
       </c>
       <c r="I9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="48" x14ac:dyDescent="0.2">
@@ -888,7 +888,7 @@
       </c>
       <c r="H10" s="6"/>
       <c r="I10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -912,7 +912,7 @@
       <c r="G11" s="4"/>
       <c r="H11" s="6"/>
       <c r="I11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="112" x14ac:dyDescent="0.2">
@@ -921,7 +921,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>17</v>
@@ -940,7 +940,7 @@
       </c>
       <c r="H12" s="6"/>
       <c r="I12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="32" x14ac:dyDescent="0.2">
@@ -964,11 +964,11 @@
         <v>0.4375</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="H13" s="6"/>
       <c r="I13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="128" x14ac:dyDescent="0.2">
@@ -977,10 +977,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="D14" s="9">
         <v>44704</v>
@@ -992,11 +992,11 @@
         <v>0.4375</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="H14" s="6"/>
       <c r="I14" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="144" x14ac:dyDescent="0.2">
@@ -1005,10 +1005,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D15" s="9">
         <v>44704</v>
@@ -1020,11 +1020,11 @@
         <v>0.4375</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H15" s="6"/>
       <c r="I15" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="48" x14ac:dyDescent="0.2">
@@ -1033,7 +1033,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="9">
@@ -1048,7 +1048,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="6"/>
       <c r="I16" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="256" x14ac:dyDescent="0.2">
@@ -1057,7 +1057,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>17</v>
@@ -1072,11 +1072,11 @@
         <v>0.51041666666666663</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H17" s="6"/>
       <c r="I17" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="80" x14ac:dyDescent="0.2">
@@ -1085,10 +1085,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D18" s="9">
         <v>44704</v>
@@ -1100,11 +1100,11 @@
         <v>0.51041666666666663</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H18" s="6"/>
       <c r="I18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="160" x14ac:dyDescent="0.2">
@@ -1113,7 +1113,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>20</v>
@@ -1128,11 +1128,11 @@
         <v>0.51041666666666663</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H19" s="6"/>
       <c r="I19" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="176" x14ac:dyDescent="0.2">
@@ -1141,10 +1141,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D20" s="9">
         <v>44704</v>
@@ -1156,11 +1156,11 @@
         <v>0.51041666666666663</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H20" s="6"/>
       <c r="I20" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -1169,7 +1169,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="9">
@@ -1186,7 +1186,7 @@
         <v>8</v>
       </c>
       <c r="I21" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="80" x14ac:dyDescent="0.2">
@@ -1195,7 +1195,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="9">
@@ -1208,13 +1208,13 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H22" s="6" t="s">
         <v>8</v>
       </c>
       <c r="I22" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="112" x14ac:dyDescent="0.2">
@@ -1223,7 +1223,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>17</v>
@@ -1238,11 +1238,11 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H23" s="6"/>
       <c r="I23" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="64" x14ac:dyDescent="0.2">
@@ -1251,7 +1251,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>20</v>
@@ -1266,11 +1266,11 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H24" s="6"/>
       <c r="I24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="176" x14ac:dyDescent="0.2">
@@ -1279,10 +1279,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D25" s="9">
         <v>44704</v>
@@ -1294,11 +1294,11 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H25" s="6"/>
       <c r="I25" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="224" x14ac:dyDescent="0.2">
@@ -1307,10 +1307,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D26" s="9">
         <v>44704</v>
@@ -1322,11 +1322,11 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="H26" s="6"/>
       <c r="I26" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="48" x14ac:dyDescent="0.2">
@@ -1335,7 +1335,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="9">
@@ -1349,10 +1349,10 @@
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I27" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -1361,7 +1361,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="9">
@@ -1376,7 +1376,7 @@
       <c r="G28" s="4"/>
       <c r="H28" s="6"/>
       <c r="I28" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -1385,7 +1385,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="9">
@@ -1402,7 +1402,7 @@
         <v>8</v>
       </c>
       <c r="I29" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -1411,7 +1411,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="9">
@@ -1425,10 +1425,10 @@
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I30" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -1454,7 +1454,7 @@
         <v>12</v>
       </c>
       <c r="I31" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -1463,7 +1463,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="9">
@@ -1480,7 +1480,7 @@
         <v>8</v>
       </c>
       <c r="I32" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="32" x14ac:dyDescent="0.2">
@@ -1489,7 +1489,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="9">
@@ -1502,13 +1502,13 @@
         <v>0.40625</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H33" s="6" t="s">
         <v>8</v>
       </c>
       <c r="I33" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="32" x14ac:dyDescent="0.2">
@@ -1517,7 +1517,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="9">
@@ -1534,7 +1534,7 @@
         <v>8</v>
       </c>
       <c r="I34" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="64" x14ac:dyDescent="0.2">
@@ -1543,7 +1543,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="9">
@@ -1560,7 +1560,7 @@
         <v>8</v>
       </c>
       <c r="I35" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -1569,7 +1569,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="9">
@@ -1586,7 +1586,7 @@
         <v>8</v>
       </c>
       <c r="I36" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -1595,7 +1595,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="9">
@@ -1612,7 +1612,7 @@
         <v>12</v>
       </c>
       <c r="I37" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added speaker entities file
</commit_message>
<xml_diff>
--- a/resources/Session Info - IBM - modified 5.7.22.xlsx
+++ b/resources/Session Info - IBM - modified 5.7.22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leighw/git/actiac/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71085DE6-B329-FF4B-A43E-BB7E03E30D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407C0000-7F16-1B41-B3D5-FC819402FC5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25580" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2440" windowWidth="25580" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -251,6 +251,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="165" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="167" formatCode="h:mm;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -314,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -330,10 +334,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="19" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,17 +622,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="26.83203125" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" customWidth="1"/>
-    <col min="5" max="5" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="21.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" style="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="54.1640625" style="7" customWidth="1"/>
     <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -641,13 +647,13 @@
       <c r="C1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="12" t="s">
         <v>60</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -668,13 +674,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="5"/>
-      <c r="D2" s="9">
+      <c r="D2" s="10">
         <v>44703</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="13">
         <v>0.35416666666666669</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="13">
         <v>0.60416666666666663</v>
       </c>
       <c r="G2" s="4"/>
@@ -692,13 +698,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="D3" s="9">
+      <c r="D3" s="10">
         <v>44703</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="13">
         <v>0.5</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="13">
         <v>0.625</v>
       </c>
       <c r="G3" s="4" t="s">
@@ -718,13 +724,13 @@
         <v>4</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="9">
+      <c r="D4" s="10">
         <v>44703</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="13">
         <v>0.6875</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="13">
         <v>0.72916666666666663</v>
       </c>
       <c r="G4" s="4"/>
@@ -742,13 +748,13 @@
         <v>5</v>
       </c>
       <c r="C5" s="5"/>
-      <c r="D5" s="9">
+      <c r="D5" s="10">
         <v>44703</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="13">
         <v>0.72916666666666663</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="13">
         <v>0.77083333333333337</v>
       </c>
       <c r="G5" s="4"/>
@@ -768,13 +774,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" s="9">
+      <c r="D6" s="10">
         <v>44703</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="13">
         <v>0.77083333333333337</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="13">
         <v>0.8125</v>
       </c>
       <c r="G6" s="4"/>
@@ -794,13 +800,13 @@
         <v>9</v>
       </c>
       <c r="C7" s="5"/>
-      <c r="D7" s="9">
+      <c r="D7" s="10">
         <v>44703</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="13">
         <v>0.8125</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="13">
         <v>0.84375</v>
       </c>
       <c r="G7" s="4" t="s">
@@ -822,13 +828,13 @@
         <v>11</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="9">
+      <c r="D8" s="10">
         <v>44703</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="13">
         <v>0.84375</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="13">
         <v>0.89583333333333337</v>
       </c>
       <c r="G8" s="4"/>
@@ -848,13 +854,13 @@
         <v>13</v>
       </c>
       <c r="C9" s="5"/>
-      <c r="D9" s="9">
-        <v>44704</v>
-      </c>
-      <c r="E9" s="12">
+      <c r="D9" s="10">
+        <v>44704</v>
+      </c>
+      <c r="E9" s="13">
         <v>0.30208333333333331</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="13">
         <v>0.34375</v>
       </c>
       <c r="G9" s="4"/>
@@ -874,13 +880,13 @@
         <v>14</v>
       </c>
       <c r="C10" s="5"/>
-      <c r="D10" s="9">
-        <v>44704</v>
-      </c>
-      <c r="E10" s="12">
+      <c r="D10" s="10">
+        <v>44704</v>
+      </c>
+      <c r="E10" s="13">
         <v>0.35416666666666669</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="13">
         <v>0.36458333333333331</v>
       </c>
       <c r="G10" s="4" t="s">
@@ -900,13 +906,13 @@
         <v>16</v>
       </c>
       <c r="C11" s="5"/>
-      <c r="D11" s="9">
-        <v>44704</v>
-      </c>
-      <c r="E11" s="12">
+      <c r="D11" s="10">
+        <v>44704</v>
+      </c>
+      <c r="E11" s="13">
         <v>0.375</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="13">
         <v>0.39583333333333331</v>
       </c>
       <c r="G11" s="4"/>
@@ -926,13 +932,13 @@
       <c r="C12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="9">
-        <v>44704</v>
-      </c>
-      <c r="E12" s="12">
+      <c r="D12" s="10">
+        <v>44704</v>
+      </c>
+      <c r="E12" s="13">
         <v>0.40625</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="13">
         <v>0.4375</v>
       </c>
       <c r="G12" s="4" t="s">
@@ -954,13 +960,13 @@
       <c r="C13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="9">
-        <v>44704</v>
-      </c>
-      <c r="E13" s="12">
+      <c r="D13" s="10">
+        <v>44704</v>
+      </c>
+      <c r="E13" s="13">
         <v>0.40625</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="13">
         <v>0.4375</v>
       </c>
       <c r="G13" s="4" t="s">
@@ -982,13 +988,13 @@
       <c r="C14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="9">
-        <v>44704</v>
-      </c>
-      <c r="E14" s="12">
+      <c r="D14" s="10">
+        <v>44704</v>
+      </c>
+      <c r="E14" s="13">
         <v>0.40625</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="13">
         <v>0.4375</v>
       </c>
       <c r="G14" s="4" t="s">
@@ -1010,13 +1016,13 @@
       <c r="C15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="9">
-        <v>44704</v>
-      </c>
-      <c r="E15" s="12">
+      <c r="D15" s="10">
+        <v>44704</v>
+      </c>
+      <c r="E15" s="13">
         <v>0.40625</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="13">
         <v>0.4375</v>
       </c>
       <c r="G15" s="4" t="s">
@@ -1036,13 +1042,13 @@
         <v>26</v>
       </c>
       <c r="C16" s="5"/>
-      <c r="D16" s="9">
-        <v>44704</v>
-      </c>
-      <c r="E16" s="12">
+      <c r="D16" s="10">
+        <v>44704</v>
+      </c>
+      <c r="E16" s="13">
         <v>0.4375</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="13">
         <v>0.46875</v>
       </c>
       <c r="G16" s="4"/>
@@ -1062,13 +1068,13 @@
       <c r="C17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="9">
-        <v>44704</v>
-      </c>
-      <c r="E17" s="12">
+      <c r="D17" s="10">
+        <v>44704</v>
+      </c>
+      <c r="E17" s="13">
         <v>0.47916666666666669</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="13">
         <v>0.51041666666666663</v>
       </c>
       <c r="G17" s="4" t="s">
@@ -1090,13 +1096,13 @@
       <c r="C18" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="9">
-        <v>44704</v>
-      </c>
-      <c r="E18" s="12">
+      <c r="D18" s="10">
+        <v>44704</v>
+      </c>
+      <c r="E18" s="13">
         <v>0.47916666666666669</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F18" s="13">
         <v>0.51041666666666663</v>
       </c>
       <c r="G18" s="4" t="s">
@@ -1118,13 +1124,13 @@
       <c r="C19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="9">
-        <v>44704</v>
-      </c>
-      <c r="E19" s="12">
+      <c r="D19" s="10">
+        <v>44704</v>
+      </c>
+      <c r="E19" s="13">
         <v>0.47916666666666669</v>
       </c>
-      <c r="F19" s="12">
+      <c r="F19" s="13">
         <v>0.51041666666666663</v>
       </c>
       <c r="G19" s="4" t="s">
@@ -1146,13 +1152,13 @@
       <c r="C20" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="9">
-        <v>44704</v>
-      </c>
-      <c r="E20" s="12">
+      <c r="D20" s="10">
+        <v>44704</v>
+      </c>
+      <c r="E20" s="13">
         <v>0.47916666666666669</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F20" s="13">
         <v>0.51041666666666663</v>
       </c>
       <c r="G20" s="4" t="s">
@@ -1172,13 +1178,13 @@
         <v>35</v>
       </c>
       <c r="C21" s="5"/>
-      <c r="D21" s="9">
-        <v>44704</v>
-      </c>
-      <c r="E21" s="12">
+      <c r="D21" s="10">
+        <v>44704</v>
+      </c>
+      <c r="E21" s="13">
         <v>0.52083333333333337</v>
       </c>
-      <c r="F21" s="12">
+      <c r="F21" s="13">
         <v>0.55208333333333337</v>
       </c>
       <c r="G21" s="4"/>
@@ -1198,13 +1204,13 @@
         <v>36</v>
       </c>
       <c r="C22" s="5"/>
-      <c r="D22" s="9">
-        <v>44704</v>
-      </c>
-      <c r="E22" s="12">
+      <c r="D22" s="10">
+        <v>44704</v>
+      </c>
+      <c r="E22" s="13">
         <v>0.55208333333333337</v>
       </c>
-      <c r="F22" s="12">
+      <c r="F22" s="13">
         <v>0.60416666666666663</v>
       </c>
       <c r="G22" s="4" t="s">
@@ -1228,13 +1234,13 @@
       <c r="C23" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="9">
-        <v>44704</v>
-      </c>
-      <c r="E23" s="12">
+      <c r="D23" s="10">
+        <v>44704</v>
+      </c>
+      <c r="E23" s="13">
         <v>0.61458333333333337</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23" s="13">
         <v>0.64583333333333337</v>
       </c>
       <c r="G23" s="4" t="s">
@@ -1256,13 +1262,13 @@
       <c r="C24" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="9">
-        <v>44704</v>
-      </c>
-      <c r="E24" s="12">
+      <c r="D24" s="10">
+        <v>44704</v>
+      </c>
+      <c r="E24" s="13">
         <v>0.61458333333333337</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24" s="13">
         <v>0.64583333333333337</v>
       </c>
       <c r="G24" s="4" t="s">
@@ -1284,13 +1290,13 @@
       <c r="C25" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="9">
-        <v>44704</v>
-      </c>
-      <c r="E25" s="12">
+      <c r="D25" s="10">
+        <v>44704</v>
+      </c>
+      <c r="E25" s="13">
         <v>0.61458333333333337</v>
       </c>
-      <c r="F25" s="12">
+      <c r="F25" s="13">
         <v>0.64583333333333337</v>
       </c>
       <c r="G25" s="4" t="s">
@@ -1312,13 +1318,13 @@
       <c r="C26" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="9">
-        <v>44704</v>
-      </c>
-      <c r="E26" s="12">
+      <c r="D26" s="10">
+        <v>44704</v>
+      </c>
+      <c r="E26" s="13">
         <v>0.61458333333333337</v>
       </c>
-      <c r="F26" s="12">
+      <c r="F26" s="13">
         <v>0.64583333333333337</v>
       </c>
       <c r="G26" s="4" t="s">
@@ -1338,13 +1344,13 @@
         <v>26</v>
       </c>
       <c r="C27" s="5"/>
-      <c r="D27" s="9">
-        <v>44704</v>
-      </c>
-      <c r="E27" s="12">
+      <c r="D27" s="10">
+        <v>44704</v>
+      </c>
+      <c r="E27" s="13">
         <v>0.64583333333333337</v>
       </c>
-      <c r="F27" s="12">
+      <c r="F27" s="13">
         <v>0.69791666666666663</v>
       </c>
       <c r="G27" s="4"/>
@@ -1364,13 +1370,13 @@
         <v>46</v>
       </c>
       <c r="C28" s="5"/>
-      <c r="D28" s="9">
-        <v>44704</v>
-      </c>
-      <c r="E28" s="12">
+      <c r="D28" s="10">
+        <v>44704</v>
+      </c>
+      <c r="E28" s="13">
         <v>0.70833333333333337</v>
       </c>
-      <c r="F28" s="12">
+      <c r="F28" s="13">
         <v>0.77083333333333337</v>
       </c>
       <c r="G28" s="4"/>
@@ -1388,13 +1394,13 @@
         <v>47</v>
       </c>
       <c r="C29" s="5"/>
-      <c r="D29" s="9">
-        <v>44704</v>
-      </c>
-      <c r="E29" s="12">
+      <c r="D29" s="10">
+        <v>44704</v>
+      </c>
+      <c r="E29" s="13">
         <v>0.77083333333333337</v>
       </c>
-      <c r="F29" s="12">
+      <c r="F29" s="13">
         <v>0.83333333333333337</v>
       </c>
       <c r="G29" s="4"/>
@@ -1414,13 +1420,13 @@
         <v>48</v>
       </c>
       <c r="C30" s="5"/>
-      <c r="D30" s="9">
-        <v>44704</v>
-      </c>
-      <c r="E30" s="12">
+      <c r="D30" s="10">
+        <v>44704</v>
+      </c>
+      <c r="E30" s="13">
         <v>0.83333333333333337</v>
       </c>
-      <c r="F30" s="12">
+      <c r="F30" s="13">
         <v>0.91666666666666663</v>
       </c>
       <c r="G30" s="4"/>
@@ -1440,13 +1446,13 @@
         <v>13</v>
       </c>
       <c r="C31" s="5"/>
-      <c r="D31" s="9">
+      <c r="D31" s="10">
         <v>44705</v>
       </c>
-      <c r="E31" s="12">
+      <c r="E31" s="13">
         <v>0.32291666666666669</v>
       </c>
-      <c r="F31" s="12">
+      <c r="F31" s="13">
         <v>0.36458333333333331</v>
       </c>
       <c r="G31" s="4"/>
@@ -1466,13 +1472,13 @@
         <v>50</v>
       </c>
       <c r="C32" s="5"/>
-      <c r="D32" s="9">
+      <c r="D32" s="10">
         <v>44705</v>
       </c>
-      <c r="E32" s="12">
+      <c r="E32" s="13">
         <v>0.35416666666666669</v>
       </c>
-      <c r="F32" s="12">
+      <c r="F32" s="13">
         <v>0.36458333333333331</v>
       </c>
       <c r="G32" s="4"/>
@@ -1492,13 +1498,13 @@
         <v>51</v>
       </c>
       <c r="C33" s="5"/>
-      <c r="D33" s="9">
+      <c r="D33" s="10">
         <v>44705</v>
       </c>
-      <c r="E33" s="12">
+      <c r="E33" s="13">
         <v>0.36458333333333331</v>
       </c>
-      <c r="F33" s="12">
+      <c r="F33" s="13">
         <v>0.40625</v>
       </c>
       <c r="G33" s="4" t="s">
@@ -1520,13 +1526,13 @@
         <v>53</v>
       </c>
       <c r="C34" s="5"/>
-      <c r="D34" s="9">
+      <c r="D34" s="10">
         <v>44705</v>
       </c>
-      <c r="E34" s="12">
+      <c r="E34" s="13">
         <v>0.40625</v>
       </c>
-      <c r="F34" s="12">
+      <c r="F34" s="13">
         <v>0.46875</v>
       </c>
       <c r="G34" s="4"/>
@@ -1546,13 +1552,13 @@
         <v>54</v>
       </c>
       <c r="C35" s="5"/>
-      <c r="D35" s="9">
+      <c r="D35" s="10">
         <v>44705</v>
       </c>
-      <c r="E35" s="12">
+      <c r="E35" s="13">
         <v>0.46875</v>
       </c>
-      <c r="F35" s="12">
+      <c r="F35" s="13">
         <v>0.5</v>
       </c>
       <c r="G35" s="4"/>
@@ -1572,13 +1578,13 @@
         <v>55</v>
       </c>
       <c r="C36" s="5"/>
-      <c r="D36" s="9">
+      <c r="D36" s="10">
         <v>44705</v>
       </c>
-      <c r="E36" s="12">
+      <c r="E36" s="13">
         <v>0.48958333333333331</v>
       </c>
-      <c r="F36" s="12">
+      <c r="F36" s="13">
         <v>0.5</v>
       </c>
       <c r="G36" s="4"/>
@@ -1598,13 +1604,13 @@
         <v>56</v>
       </c>
       <c r="C37" s="5"/>
-      <c r="D37" s="9">
+      <c r="D37" s="10">
         <v>44705</v>
       </c>
-      <c r="E37" s="12">
+      <c r="E37" s="13">
         <v>0.5</v>
       </c>
-      <c r="F37" s="12">
+      <c r="F37" s="13">
         <v>0.5</v>
       </c>
       <c r="G37" s="4"/>

</xml_diff>

<commit_message>
adjustments to session descriptions
</commit_message>
<xml_diff>
--- a/resources/Session Info - IBM - modified 5.7.22.xlsx
+++ b/resources/Session Info - IBM - modified 5.7.22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leighw/git/actiac/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407C0000-7F16-1B41-B3D5-FC819402FC5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{574553C5-8BEB-344D-8BA5-A68A258509C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2440" windowWidth="25580" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1680" windowWidth="25580" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -121,9 +121,6 @@
     <t>Discover Digital Transformation Powered by Emerging Technologies: Local to Global Perspectives</t>
   </si>
   <si>
-    <t>Emerging technologies are accelerators of innovation. They can improve efficiency, power new products and services, enable new business models, and reinvent governments &amp; businesses for the benefit of citizens and consumers alike. More and more, the world is becoming digital. Every successful enterprise will one day be a digital enterprise. How are leading companies and governments making this journey? During this session, government and industry executives — from the U.S. and internationally — will detail the digital reinvention of their organizations to better serve citizens and consumers in this digital age. They will share how they are taking advantage of new opportunities in AI &amp; automation, robotics, blockchain, 5G, with the reach of cloud and edge and the assurance of cyber, to data-analytics and other areas to transform their organizations, engineer a competitive advantage, and ultimately help governments and businesses enable more efficient, responsive systems to enhance customer experience and accelerate progress.</t>
-  </si>
-  <si>
     <t>Healthcare Reimagined:  Merging the Physical and Digital</t>
   </si>
   <si>
@@ -133,9 +130,6 @@
     <t>Managing the Multicloud Future</t>
   </si>
   <si>
-    <t>As more and more workloads move to the cloud, government agencies are grappling with how to offer cloud services efficiently while maintaining maximum choice for individual programs. Giving more choice to programs through IDIQs, and other contract vehicles, means that agency and government leaders and must work across programs to make sure that data does not stay siloed and is shared across agencies and across the federal government. Multi-cloud management is critical to sharing and securing data as agencies continue to move to a distributed cloud approach, taking advantage of edge and 5g technologies.</t>
-  </si>
-  <si>
     <t>The Future Relies on Collaborative Innovation of Digital Supply Chains Across Mission Ecosystems</t>
   </si>
   <si>
@@ -245,6 +239,12 @@
   </si>
   <si>
     <t>What if R O I was not in a spreadsheet or financial ledger, but it was the constituent experience and the satisfaction of a job done well. Not just well done even - amazingly done. We, with a partnership of industry and public sector, must focus on the experience of the actual people we need to serve and reduce the burden on our public sector workforce.  State governments are harnessing the momentum of change to focus on the citizen experience and enabling agencies to innovate and modernize the way we serve customers. State agencies are propelling the path to production, while Central I T is utilizing strategic technologies to empower agencies to act faster and mitigate the unforeseen risk inherent in I T operations.  How do we realize Public R O I? By removing the barriers to innovation, owning the hurdles that slow operations down and embracing the momentum of change.</t>
+  </si>
+  <si>
+    <t>As more and more workloads move to the cloud, government agencies are grappling with how to offer cloud services efficiently while maintaining maximum choice for individual programs. Giving more choice to programs through IDIQs, and other contract vehicles, means that agency and government leaders must work across programs to make sure that data does not stay siloed and is shared across agencies and across the federal government. Multi-cloud management is critical to sharing and securing data as agencies continue to move to a distributed cloud approach, taking advantage of edge and 5g technologies.</t>
+  </si>
+  <si>
+    <t>Emerging technologies are accelerators of innovation. They can improve efficiency, power new products and services, enable new business models, and reinvent governments &amp; businesses for the benefit of citizens and consumers alike. More and more, the world is becoming digital. Every successful enterprise will one day be a digital enterprise. How are leading companies and governments making this journey? During this session, government and industry executives — from the U S and internationally — will detail the digital reinvention of their organizations to better serve citizens and consumers in this digital age. They will share how they are taking advantage of new opportunities in A I and automation, robotics, blockchain, 5G, with the reach of cloud and edge, and the assurance of cyber, to data-analytics and other areas to transform their organizations, engineer a competitive advantage, and ultimately help governments and businesses enable more efficient, responsive systems to enhance customer experience and accelerate progress.</t>
   </si>
 </sst>
 </file>
@@ -622,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -639,31 +639,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>58</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>60</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -686,7 +686,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="32" x14ac:dyDescent="0.2">
@@ -712,7 +712,7 @@
       </c>
       <c r="H3" s="6"/>
       <c r="I3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -736,7 +736,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="6"/>
       <c r="I4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -762,7 +762,7 @@
         <v>6</v>
       </c>
       <c r="I5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -788,7 +788,7 @@
         <v>8</v>
       </c>
       <c r="I6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="48" x14ac:dyDescent="0.2">
@@ -816,7 +816,7 @@
         <v>8</v>
       </c>
       <c r="I7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -842,7 +842,7 @@
         <v>12</v>
       </c>
       <c r="I8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -868,7 +868,7 @@
         <v>12</v>
       </c>
       <c r="I9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="48" x14ac:dyDescent="0.2">
@@ -894,7 +894,7 @@
       </c>
       <c r="H10" s="6"/>
       <c r="I10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -918,7 +918,7 @@
       <c r="G11" s="4"/>
       <c r="H11" s="6"/>
       <c r="I11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="112" x14ac:dyDescent="0.2">
@@ -927,7 +927,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>17</v>
@@ -946,7 +946,7 @@
       </c>
       <c r="H12" s="6"/>
       <c r="I12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="32" x14ac:dyDescent="0.2">
@@ -970,11 +970,11 @@
         <v>0.4375</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H13" s="6"/>
       <c r="I13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="128" x14ac:dyDescent="0.2">
@@ -998,11 +998,11 @@
         <v>0.4375</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H14" s="6"/>
       <c r="I14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="144" x14ac:dyDescent="0.2">
@@ -1030,7 +1030,7 @@
       </c>
       <c r="H15" s="6"/>
       <c r="I15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="48" x14ac:dyDescent="0.2">
@@ -1054,7 +1054,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="6"/>
       <c r="I16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="256" x14ac:dyDescent="0.2">
@@ -1078,11 +1078,11 @@
         <v>0.51041666666666663</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="H17" s="6"/>
       <c r="I17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="80" x14ac:dyDescent="0.2">
@@ -1091,7 +1091,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>24</v>
@@ -1106,11 +1106,11 @@
         <v>0.51041666666666663</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H18" s="6"/>
       <c r="I18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="160" x14ac:dyDescent="0.2">
@@ -1119,7 +1119,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>20</v>
@@ -1134,11 +1134,11 @@
         <v>0.51041666666666663</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="H19" s="6"/>
       <c r="I19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="176" x14ac:dyDescent="0.2">
@@ -1147,7 +1147,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>22</v>
@@ -1162,11 +1162,11 @@
         <v>0.51041666666666663</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H20" s="6"/>
       <c r="I20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -1175,7 +1175,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="10">
@@ -1192,7 +1192,7 @@
         <v>8</v>
       </c>
       <c r="I21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="80" x14ac:dyDescent="0.2">
@@ -1201,7 +1201,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="10">
@@ -1214,13 +1214,13 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H22" s="6" t="s">
         <v>8</v>
       </c>
       <c r="I22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="112" x14ac:dyDescent="0.2">
@@ -1229,7 +1229,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>17</v>
@@ -1244,11 +1244,11 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H23" s="6"/>
       <c r="I23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="64" x14ac:dyDescent="0.2">
@@ -1257,7 +1257,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>20</v>
@@ -1272,11 +1272,11 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H24" s="6"/>
       <c r="I24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="176" x14ac:dyDescent="0.2">
@@ -1285,7 +1285,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>24</v>
@@ -1300,11 +1300,11 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H25" s="6"/>
       <c r="I25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="224" x14ac:dyDescent="0.2">
@@ -1313,7 +1313,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>22</v>
@@ -1328,11 +1328,11 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H26" s="6"/>
       <c r="I26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="48" x14ac:dyDescent="0.2">
@@ -1355,10 +1355,10 @@
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I27" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -1367,7 +1367,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="10">
@@ -1382,7 +1382,7 @@
       <c r="G28" s="4"/>
       <c r="H28" s="6"/>
       <c r="I28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -1391,7 +1391,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="10">
@@ -1408,7 +1408,7 @@
         <v>8</v>
       </c>
       <c r="I29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -1417,7 +1417,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="10">
@@ -1431,10 +1431,10 @@
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -1460,7 +1460,7 @@
         <v>12</v>
       </c>
       <c r="I31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -1469,7 +1469,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="10">
@@ -1486,7 +1486,7 @@
         <v>8</v>
       </c>
       <c r="I32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="32" x14ac:dyDescent="0.2">
@@ -1495,7 +1495,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="10">
@@ -1508,13 +1508,13 @@
         <v>0.40625</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H33" s="6" t="s">
         <v>8</v>
       </c>
       <c r="I33" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="32" x14ac:dyDescent="0.2">
@@ -1523,7 +1523,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="10">
@@ -1540,7 +1540,7 @@
         <v>8</v>
       </c>
       <c r="I34" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="64" x14ac:dyDescent="0.2">
@@ -1549,7 +1549,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="10">
@@ -1566,7 +1566,7 @@
         <v>8</v>
       </c>
       <c r="I35" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -1575,7 +1575,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="10">
@@ -1592,7 +1592,7 @@
         <v>8</v>
       </c>
       <c r="I36" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -1601,7 +1601,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="10">
@@ -1618,7 +1618,7 @@
         <v>12</v>
       </c>
       <c r="I37" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>